<commit_message>
Second commit of DB Homework 1
</commit_message>
<xml_diff>
--- a/1 семенар/HomeWork1.xlsx
+++ b/1 семенар/HomeWork1.xlsx
@@ -23,9 +23,163 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+  <si>
+    <t>Составьте таблицы для хранения сведений об общественном транспорте.
+— Можно на примере автобусов.
+— При составлении таблиц не берите слишком много сущностей. Ориентируйтесь на структуру типа: «У нас есть автобусы на разных маршрутах, у автобуса есть водитель, также в автобусе работает кондуктор». Более сложные/глубокие структуры пока лучше не брать.</t>
+  </si>
+  <si>
+    <t>Автобусы</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ID_Марка</t>
+  </si>
+  <si>
+    <t>ID_Маршрута</t>
+  </si>
+  <si>
+    <t>Маршруты</t>
+  </si>
+  <si>
+    <t>Остановки</t>
+  </si>
+  <si>
+    <t>Номер</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Адрес</t>
+  </si>
+  <si>
+    <t>ID_Остановки</t>
+  </si>
+  <si>
+    <t>№_Остановки_в_маршруте</t>
+  </si>
+  <si>
+    <t>ID_Депо</t>
+  </si>
+  <si>
+    <t>ID_Маршрут</t>
+  </si>
+  <si>
+    <t>Депо</t>
+  </si>
+  <si>
+    <t>Время начала движения</t>
+  </si>
+  <si>
+    <t>Время окончания движения</t>
+  </si>
+  <si>
+    <t>Интервал движения</t>
+  </si>
+  <si>
+    <t>Телефон</t>
+  </si>
+  <si>
+    <t>Дата_Техосмотра</t>
+  </si>
+  <si>
+    <t>Марка</t>
+  </si>
+  <si>
+    <t>Производитель</t>
+  </si>
+  <si>
+    <t>Модель</t>
+  </si>
+  <si>
+    <t>Вместимость</t>
+  </si>
+  <si>
+    <t>Сотрудники</t>
+  </si>
+  <si>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>Серия</t>
+  </si>
+  <si>
+    <t>Дата выдачи</t>
+  </si>
+  <si>
+    <t>Дата окончания действия</t>
+  </si>
+  <si>
+    <t>ID_Тип_документа</t>
+  </si>
+  <si>
+    <t>Наименование</t>
+  </si>
+  <si>
+    <t>ID_Сотрудника</t>
+  </si>
+  <si>
+    <t>ID_Документа</t>
+  </si>
+  <si>
+    <t>ID_Автобуса</t>
+  </si>
+  <si>
+    <t>ID_Водитель</t>
+  </si>
+  <si>
+    <t>ID_Кондуктор</t>
+  </si>
+  <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>Кем выдан</t>
+  </si>
+  <si>
+    <t>Работает?</t>
+  </si>
+  <si>
+    <t>Отделы</t>
+  </si>
+  <si>
+    <t>ID_Начальника</t>
+  </si>
+  <si>
+    <t>Номерной_знак</t>
+  </si>
+  <si>
+    <t>Контактный_телефон</t>
+  </si>
+  <si>
+    <t>ID_Отдела</t>
+  </si>
+  <si>
+    <t>Документы_сотрудников</t>
+  </si>
+  <si>
+    <t>Тип_документа</t>
+  </si>
+  <si>
+    <t>Промежуточная_Маршрут_Остановка</t>
+  </si>
+  <si>
+    <t>Лог_Автобусы_Маршруты_Водители_Кондукторы_Дата</t>
+  </si>
+  <si>
+    <t>Промежуточная_Сотрудник_Документ</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +188,50 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -51,12 +239,422 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -337,12 +935,513 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31:L31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
+    <col min="2" max="2" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="I12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="27"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="17" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="H18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24"/>
+      <c r="L18" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" s="23"/>
+      <c r="N18" s="24"/>
+    </row>
+    <row r="19" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="N19" s="42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="21"/>
+    </row>
+    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="18"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="18"/>
+    </row>
+    <row r="23" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="G24" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="J24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="27"/>
+    </row>
+    <row r="25" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="O25" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="21"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="21"/>
+    </row>
+    <row r="27" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="18"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="18"/>
+    </row>
+    <row r="29" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
+      <c r="K30" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="27"/>
+    </row>
+    <row r="31" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="21"/>
+    </row>
+    <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="38" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G39" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="12"/>
+    </row>
+    <row r="40" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G40" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L40" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G41" s="13"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="15"/>
+    </row>
+    <row r="42" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G42" s="16"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="A1:Q5"/>
+    <mergeCell ref="G39:L39"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="K30:L30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>